<commit_message>
Ajustes en validaciones y lógica de ReclutarCandidato
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanCamiloAnaconaMaz\Downloads\Reto_Tecnico-Choucair-master\Reto_Tecnico-Choucair-master\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE21510-17BE-470D-88A1-C8FB748AC6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037694E4-04D7-4014-AF24-6D3C370374B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosIngreso" sheetId="5" r:id="rId1"/>
     <sheet name="FormularioCandidato" sheetId="4" r:id="rId2"/>
     <sheet name="Entrevista" sheetId="6" r:id="rId3"/>
-    <sheet name="Validacion" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>admin123</t>
   </si>
@@ -97,30 +96,6 @@
   </si>
   <si>
     <t>juancamiloanacondamazabel@gmail.com</t>
-  </si>
-  <si>
-    <t>Vacancy</t>
-  </si>
-  <si>
-    <t>Candidate</t>
-  </si>
-  <si>
-    <t>Hiring Manager</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Juan Camilo Anacona</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Rahul Mulge Patil</t>
-  </si>
-  <si>
-    <t>Hired</t>
   </si>
 </sst>
 </file>
@@ -556,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CE2614-FDAD-45BB-B8B4-AE1B64F22021}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -592,52 +567,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85AA20C-293F-443A-A10C-8BF0119103AB}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización de lógica en ValidarValoresQuestions, VerificarTextoEnTabla y reclutamiento
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanCamiloAnaconaMaz\Downloads\Reto_Tecnico-Choucair-master\Reto_Tecnico-Choucair-master\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037694E4-04D7-4014-AF24-6D3C370374B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B259029-9E95-4948-9BE1-E75BAC789ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosIngreso" sheetId="5" r:id="rId1"/>
     <sheet name="FormularioCandidato" sheetId="4" r:id="rId2"/>
     <sheet name="Entrevista" sheetId="6" r:id="rId3"/>
+    <sheet name="Validacion" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>admin123</t>
   </si>
@@ -96,6 +97,24 @@
   </si>
   <si>
     <t>juancamiloanacondamazabel@gmail.com</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Payroll Administrator</t>
+  </si>
+  <si>
+    <t>Juan Camilo Anacona</t>
+  </si>
+  <si>
+    <t>Hired</t>
   </si>
 </sst>
 </file>
@@ -458,12 +477,12 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15.7265625" customWidth="1"/>
     <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.81640625" customWidth="1"/>
@@ -531,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CE2614-FDAD-45BB-B8B4-AE1B64F22021}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -567,4 +586,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BF21C9-73B1-4C89-A5FF-470C53A4DA0F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>